<commit_message>
before using angular-bootstrap ui
</commit_message>
<xml_diff>
--- a/Document/notes.xlsx
+++ b/Document/notes.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">merge (keyword:keyword {keyword:'"+note.keyword+"'}) </t>
   </si>
   <si>
-    <t xml:space="preserve">merge (date:date {date:today}) </t>
+    <t xml:space="preserve">merge (date:date {date:'"+today+"'}) </t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
-        <v>+"merge (date:date {date:today}) "</v>
+        <v>+"merge (date:date {date:'"+today+"'}) "</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,15 +680,15 @@
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
-        <v>"create (note)-[linkTo:linkTo]-&gt;(keyword) "</v>
+        <v>+"create (note)-[linkTo:linkTo]-&gt;(keyword) "</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
display by select calendar date
</commit_message>
<xml_diff>
--- a/Document/notes.xlsx
+++ b/Document/notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cypher" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t xml:space="preserve">match  (note:note)-[createdOn:createdOn]-&gt;(date) </t>
   </si>
@@ -87,12 +87,6 @@
     <t xml:space="preserve">merge (date:date {date:'"+today+"'}) </t>
   </si>
   <si>
-    <t>match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '开心'</t>
-  </si>
-  <si>
-    <t>match (note) where note.details CONTAINS '西瓜'</t>
-  </si>
-  <si>
     <t>match (note)-[createdBy:createdBy]-(creator:user)</t>
   </si>
   <si>
@@ -106,19 +100,40 @@
   </si>
   <si>
     <t>match (note)-[aboutUser:aboutUser]-&gt;(aboutwho:user) where aboutwho.email=' "+para.about+"'</t>
+  </si>
+  <si>
+    <t>match (note) where note.details CONTAINS '"+para.detail+"'</t>
+  </si>
+  <si>
+    <t>match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '"+para.keyword+"'</t>
+  </si>
+  <si>
+    <t>match (keyword:keyword) where keyword.keyword contains '"+req.body.keyword+"' return keyword.keyword</t>
+  </si>
+  <si>
+    <t>give family id in the url to display home picture</t>
+  </si>
+  <si>
+    <t>if not, use default one, and show how many families have setuo their own board, and care about their data of life</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF525864"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D36"/>
+  <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +775,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -774,7 +790,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>4</v>
@@ -789,7 +805,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>4</v>
@@ -799,27 +815,27 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="2"/>
-        <v>+"match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '开心'"</v>
+        <v>+"match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '"+para.keyword+"'"</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" ref="D33:D36" si="3">B33&amp;A33&amp;C33</f>
-        <v>"match (note) where note.details CONTAINS '西瓜'"</v>
+        <v>+"match (note) where note.details CONTAINS '"+para.detail+"'"</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
@@ -834,7 +850,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>4</v>
@@ -849,7 +865,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -862,19 +878,48 @@
         <v>"order by aboutwho.firstname, keyword.keyword, creator.firstname, note.details ",</v>
       </c>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" ref="D43" si="4">B43&amp;A43&amp;C43</f>
+        <v>"match (keyword:keyword) where keyword.keyword contains '"+req.body.keyword+"' return keyword.keyword",</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
count on keywords on search done
</commit_message>
<xml_diff>
--- a/Document/notes.xlsx
+++ b/Document/notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t xml:space="preserve">match  (note:note)-[createdOn:createdOn]-&gt;(date) </t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>if not, use default one, and show how many families have setuo their own board, and care about their data of life</t>
+  </si>
+  <si>
+    <t>some topped used keywords display one login page</t>
   </si>
 </sst>
 </file>
@@ -901,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,6 +920,11 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
family members dropdown list
</commit_message>
<xml_diff>
--- a/Document/notes.xlsx
+++ b/Document/notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="cypher" sheetId="1" r:id="rId1"/>
@@ -16,16 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
-  <si>
-    <t xml:space="preserve">match  (note:note)-[createdOn:createdOn]-&gt;(date) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">match  (note)-[link:linkTo]-&gt;(keyword:keyword) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">match  (note)-[create:createdBy]-&gt;(creator:user) </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>"</t>
   </si>
@@ -33,18 +24,6 @@
     <t>+"</t>
   </si>
   <si>
-    <t xml:space="preserve">match  (note)-[about:aboutUser]-&gt;(members) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">return {about:members.firstname,creator:creator.firstname, keyword:keyword.keyword, details:note.details}  as note </t>
-  </si>
-  <si>
-    <t xml:space="preserve">order by members.firstname, keyword.keyword, creator.firstname, note.details </t>
-  </si>
-  <si>
-    <t xml:space="preserve">match  (login)-[f1:userBelongToFamily]-&gt;(f:family) </t>
-  </si>
-  <si>
     <t xml:space="preserve">match  (members:user)-[f2:userBelongToFamily]-&gt;(f) </t>
   </si>
   <si>
@@ -54,9 +33,6 @@
     <t xml:space="preserve">match  (login:user {email:'"+loginUser+"'}) </t>
   </si>
   <si>
-    <t xml:space="preserve">match  (date:date {date:'"+today+"'}) </t>
-  </si>
-  <si>
     <t xml:space="preserve">match (creator:user {email:'"+loginUser+"'}) </t>
   </si>
   <si>
@@ -108,9 +84,6 @@
     <t>match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '"+para.keyword+"'</t>
   </si>
   <si>
-    <t>match (keyword:keyword) where keyword.keyword contains '"+req.body.keyword+"' return keyword.keyword</t>
-  </si>
-  <si>
     <t>give family id in the url to display home picture</t>
   </si>
   <si>
@@ -118,6 +91,21 @@
   </si>
   <si>
     <t>some topped used keywords display one login page</t>
+  </si>
+  <si>
+    <t>List Note from date</t>
+  </si>
+  <si>
+    <t>Search notes in date range</t>
+  </si>
+  <si>
+    <t>Family members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">match (login)-[r:userBelongToFamily]-&gt;(f) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">return members </t>
   </si>
 </sst>
 </file>
@@ -133,18 +121,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF525864"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +158,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D43"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,424 +472,334 @@
     <col min="4" max="4" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="str">
-        <f>B2&amp;A2&amp;C2</f>
-        <v>"match  (login:user {email:'"+loginUser+"'}) "</v>
+        <f t="shared" ref="D2:D11" si="0">B2&amp;A2&amp;C2</f>
+        <v>"match (creator:user {email:'"+loginUser+"'}) "</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D11" si="0">B3&amp;A3&amp;C3</f>
-        <v>+"match  (login)-[f1:userBelongToFamily]-&gt;(f:family) "</v>
+        <f t="shared" si="0"/>
+        <v>+"match (tagged:user {email:'"+note.about+"'}) "</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>+"match  (members:user)-[f2:userBelongToFamily]-&gt;(f) "</v>
+        <v>+"merge (keyword:keyword {keyword:'"+note.keyword+"'}) "</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>+"match  (date:date {date:'"+today+"'}) "</v>
+        <v>+"merge (tagged)-[feel:feel]-&gt;(keyword) "</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>+"match  (note:note)-[createdOn:createdOn]-&gt;(date) "</v>
+        <v>+"merge (date:date {date:'"+today+"'}) "</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>+"match  (note)-[about:aboutUser]-&gt;(members) "</v>
+        <v>+"create (note:note {details:'"+note.detail+"', value:'"+note.value+"'}) "</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>+"match  (note)-[link:linkTo]-&gt;(keyword:keyword) "</v>
+        <v>+"create (note)-[linkTo:linkTo]-&gt;(keyword) "</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>+"match  (note)-[create:createdBy]-&gt;(creator:user) "</v>
+        <v>+"create (note)-[createdBy:createdBy]-&gt;(creator) "</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>+"return {about:members.firstname,creator:creator.firstname, keyword:keyword.keyword, details:note.details}  as note "</v>
+        <v>+"create (note)-[aboutUser:aboutUser]-&gt;(tagged) "</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>+"order by members.firstname, keyword.keyword, creator.firstname, note.details ",</v>
+        <v>+"create (note)-[createdOn:createdOn {time:timestamp()}]-&gt;(date) ",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" ref="D14:D16" si="1">B14&amp;A14&amp;C14</f>
+        <v>"match (note:note)-[createdOn:createdOn]-&gt;(date:date) where date.date &gt;='"+para.from+"' AND date.date&lt;='"+para.to+"' "</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>+"match (note)-[aboutUser:aboutUser]-&gt;(aboutwho:user) where aboutwho.email=' "+para.about+"'"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>+"match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '"+para.keyword+"'"</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D17:D26" si="1">B17&amp;A17&amp;C17</f>
-        <v>"match (creator:user {email:'"+loginUser+"'}) "</v>
+        <f t="shared" ref="D17:D20" si="2">B17&amp;A17&amp;C17</f>
+        <v>+"match (note) where note.details CONTAINS '"+para.detail+"'"</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="1"/>
-        <v>+"match (tagged:user {email:'"+note.about+"'}) "</v>
+        <f t="shared" si="2"/>
+        <v>+"match (note)-[createdBy:createdBy]-(creator:user)"</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="1"/>
-        <v>+"merge (keyword:keyword {keyword:'"+note.keyword+"'}) "</v>
+        <f t="shared" si="2"/>
+        <v>+"return {about:aboutwho.firstname,creator:creator.firstname, keyword:keyword.keyword, details:note.details,createdOn:date.date}  as result "</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="1"/>
-        <v>+"merge (tagged)-[feel:feel]-&gt;(keyword) "</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="1"/>
-        <v>+"merge (date:date {date:'"+today+"'}) "</v>
+        <f t="shared" si="2"/>
+        <v>"order by aboutwho.firstname, keyword.keyword, creator.firstname, note.details ",</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="1"/>
-        <v>+"create (note:note {details:'"+note.detail+"', value:'"+note.value+"'}) "</v>
+      <c r="A22" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="1"/>
-        <v>+"create (note)-[linkTo:linkTo]-&gt;(keyword) "</v>
+        <f t="shared" ref="D23:D24" si="3">B23&amp;A23&amp;C23</f>
+        <v>"match  (login:user {email:'"+loginUser+"'}) "</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="1"/>
-        <v>+"create (note)-[createdBy:createdBy]-&gt;(creator) "</v>
+        <f t="shared" si="3"/>
+        <v>+"match (login)-[r:userBelongToFamily]-&gt;(f) "</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="1"/>
-        <v>+"create (note)-[aboutUser:aboutUser]-&gt;(tagged) "</v>
+        <f t="shared" ref="D25" si="4">B25&amp;A25&amp;C25</f>
+        <v>+"match  (members:user)-[f2:userBelongToFamily]-&gt;(f) "</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="1"/>
-        <v>+"create (note)-[createdOn:createdOn {time:timestamp()}]-&gt;(date) ",</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" ref="D30:D32" si="2">B30&amp;A30&amp;C30</f>
-        <v>"match (note:note)-[createdOn:createdOn]-&gt;(date:date) where date.date &gt;='"+para.from+"' AND date.date&lt;='"+para.to+"' "</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="2"/>
-        <v>+"match (note)-[aboutUser:aboutUser]-&gt;(aboutwho:user) where aboutwho.email=' "+para.about+"'"</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="2"/>
-        <v>+"match (note)-[linkTo:linkTo]-&gt;(keyword:keyword) where keyword.keyword CONTAINS '"+para.keyword+"'"</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" ref="D33:D36" si="3">B33&amp;A33&amp;C33</f>
-        <v>+"match (note) where note.details CONTAINS '"+para.detail+"'"</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="3"/>
-        <v>+"match (note)-[createdBy:createdBy]-(creator:user)"</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="3"/>
-        <v>+"return {about:aboutwho.firstname,creator:creator.firstname, keyword:keyword.keyword, details:note.details,createdOn:date.date}  as result "</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="3"/>
-        <v>"order by aboutwho.firstname, keyword.keyword, creator.firstname, note.details ",</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" ref="D43" si="4">B43&amp;A43&amp;C43</f>
-        <v>"match (keyword:keyword) where keyword.keyword contains '"+req.body.keyword+"' return keyword.keyword",</v>
+        <f t="shared" ref="D26" si="5">B26&amp;A26&amp;C26</f>
+        <v>+"return members ",</v>
       </c>
     </row>
   </sheetData>
@@ -906,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -914,17 +820,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>